<commit_message>
[mrp_compoennt_impot] fix report xlsx issue
</commit_message>
<xml_diff>
--- a/carpentry_mrp_import/report/report_mrp_component_unknown.xlsx
+++ b/carpentry_mrp_import/report/report_mrp_component_unknown.xlsx
@@ -2,82 +2,62 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/755d17a41cebba5b/Documents/Dev/odoo-community-carpentry/carpentry_mrp_import/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{66E050DF-7E46-4194-9983-7BF5E0D7CD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D06AD923-989D-4CE0-B671-6E09B76FDC61}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729DB1C-0E3F-4F39-9F2F-2535A56C09A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32415" yWindow="2400" windowWidth="18000" windowHeight="9210" xr2:uid="{84DCFFFE-D3A6-43CC-B9D0-ADD080F227AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit of Measure</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
   <si>
     <t>Manufacturing Order</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>default_code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>uom_name</t>
-  </si>
-  <si>
-    <t>price * discount</t>
-  </si>
-  <si>
-    <t>product_uom_qty</t>
-  </si>
-  <si>
-    <t>Unknown products during Manufacturing Components import</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Unknown products of Manufacturing Components import</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,12 +107,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,61 +466,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB3976E-235B-4739-8BA1-FF73FCD6C27B}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="6" width="14" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10">
+        <v>45292</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'security/carpentry_position_budget_security.xml', bug fix security
</commit_message>
<xml_diff>
--- a/carpentry_mrp_import/report/report_mrp_component_unknown.xlsx
+++ b/carpentry_mrp_import/report/report_mrp_component_unknown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/755d17a41cebba5b/Documents/Dev/odoo-community-carpentry/carpentry_mrp_import/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729DB1C-0E3F-4F39-9F2F-2535A56C09A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{4729DB1C-0E3F-4F39-9F2F-2535A56C09A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{290B21D0-BCC9-4FE0-818C-D1BFCDD8578B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-1632" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Reference</t>
   </si>
@@ -46,7 +46,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Unknown products of Manufacturing Components import</t>
+    <t>Section title</t>
+  </si>
+  <si>
+    <t>Report for the import of manufacturing Components</t>
   </si>
 </sst>
 </file>
@@ -56,9 +59,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +82,14 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -107,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -120,8 +131,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -131,6 +142,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -467,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +499,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -515,20 +529,25 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>